<commit_message>
Removing any reference on tweets or epitweetr
</commit_message>
<xml_diff>
--- a/episomer/inst/extdata/geo-training.xlsx
+++ b/episomer/inst/extdata/geo-training.xlsx
@@ -46,22 +46,22 @@
     <t xml:space="preserve">Source</t>
   </si>
   <si>
-    <t xml:space="preserve">Tweet Id</t>
+    <t xml:space="preserve">Post Id</t>
   </si>
   <si>
     <t xml:space="preserve">Lang</t>
   </si>
   <si>
-    <t xml:space="preserve">Tweet part</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Epitweetr match</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Epitweetr country match</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Epitweetr country code match</t>
+    <t xml:space="preserve">Post part</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Episomer match</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Episomer country match</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Episomer country code match</t>
   </si>
   <si>
     <t xml:space="preserve">Demonym</t>
@@ -8612,6 +8612,43 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF860D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFDE59"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF7D1D5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDEDCE6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -8687,10 +8724,10 @@
   <dimension ref="A1:M2637"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.48"/>
@@ -56210,7 +56247,7 @@
   <autoFilter ref="A1:M2637"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>